<commit_message>
adding fex_max_recording_exo and updated gpr models
</commit_message>
<xml_diff>
--- a/data/CollectionPoints.xlsx
+++ b/data/CollectionPoints.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\FES_Exo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{086C2665-DB6C-439E-92BB-C32B867C1984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CBA38E4A-A4ED-4368-AAC7-92BCCB61C405}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Bicep, Tricep</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ElbowFE</t>
   </si>
@@ -41,14 +37,11 @@
   <si>
     <t>WristRU</t>
   </si>
-  <si>
-    <t>Others</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,11 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,20 +386,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA674AA-4F97-4701-B0BE-B460A79DCC22}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.21875" customWidth="1"/>
+    <col min="1" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -419,12 +411,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
@@ -434,106 +423,99 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -541,46 +523,41 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -588,57 +565,53 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
       <c r="B16">
         <v>1</v>
       </c>
@@ -646,14 +619,13 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
       <c r="B17">
         <v>1</v>
       </c>
@@ -661,47 +633,122 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A19"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>